<commit_message>
Se añadio a Zulma
</commit_message>
<xml_diff>
--- a/A_2023_2_GIT (lista de grupos).xlsx
+++ b/A_2023_2_GIT (lista de grupos).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rogerruizescobar/Documents/2023-1_Sistemas de Infromacion y Sistemas Inteligentes/2023-2/Grupo A/UDABOL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9212965-B09D-7A4D-9385-EED80DF29B22}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90B0F35A-9ABB-C740-BCC7-FC49CCD5DCD0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Respuestas de formulario 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="71">
   <si>
     <t>Paterno</t>
   </si>
@@ -227,6 +227,12 @@
   </si>
   <si>
     <t>grupo</t>
+  </si>
+  <si>
+    <t>Rocha</t>
+  </si>
+  <si>
+    <t>Zulma Clara</t>
   </si>
 </sst>
 </file>
@@ -517,11 +523,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="A1:B1048576"/>
+      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -853,6 +859,20 @@
         <v>2</v>
       </c>
     </row>
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>